<commit_message>
Implement L3 process details mapping and enhance process flow visualization
- Added a new function to build a lookup map of L3 process names to their details (objective, use_case, it_release) for improved data enrichment.
- Integrated the L3 details map into the process flow visualization, allowing for enriched node data display.
- Updated the legend in the process flow view to dynamically reflect actual Value Stream names from the data.
- Enhanced the import functionality to rebuild the L3 lookup map when new hierarchy data is loaded.
- Refactored the parseDependencies function to support optional enrichment with L3 details, improving data consistency and clarity.
</commit_message>
<xml_diff>
--- a/Connections.xlsx
+++ b/Connections.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eyus-my.sharepoint.com/personal/tony_calabro_ey_com/Documents/Desktop/Cursor/Hierarchy 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="8_{A326F537-9C9C-4DE6-A793-9A61B1FAA38A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C310C676-E1DE-4624-A18B-AB21C82AD308}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="8_{A326F537-9C9C-4DE6-A793-9A61B1FAA38A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC3E6FF6-3F2F-41B7-8AE7-37F1CEC831BF}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C5CF7D8D-18C1-4DA6-BBC5-CBC3C1BDFBAD}"/>
   </bookViews>
   <sheets>
     <sheet name="Connections" sheetId="7" r:id="rId1"/>
+    <sheet name="Previous Update v4" sheetId="8" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Connections!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Previous Update v4'!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="188">
   <si>
     <t>Plan and Procure Metering Assets</t>
   </si>
@@ -594,6 +596,15 @@
   </si>
   <si>
     <t>Tamper/Fail Alarm</t>
+  </si>
+  <si>
+    <t>Suspect Usage Flag</t>
+  </si>
+  <si>
+    <t>Confirmed Theft Case</t>
+  </si>
+  <si>
+    <t>Grid Asset Alarm</t>
   </si>
 </sst>
 </file>
@@ -974,9 +985,1557 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16457C1E-DB35-46F2-9BC1-E2CF8C3A2E02}">
+  <dimension ref="A1:D109"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:XFD24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="59.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>144</v>
+      </c>
+      <c r="D3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" t="s">
+        <v>145</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" t="s">
+        <v>173</v>
+      </c>
+      <c r="D8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>146</v>
+      </c>
+      <c r="D12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>174</v>
+      </c>
+      <c r="D13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" t="s">
+        <v>109</v>
+      </c>
+      <c r="C14" t="s">
+        <v>147</v>
+      </c>
+      <c r="D14" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" t="s">
+        <v>109</v>
+      </c>
+      <c r="C15" t="s">
+        <v>148</v>
+      </c>
+      <c r="D15" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C16" t="s">
+        <v>149</v>
+      </c>
+      <c r="D16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" t="s">
+        <v>108</v>
+      </c>
+      <c r="C17" t="s">
+        <v>150</v>
+      </c>
+      <c r="D17" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" t="s">
+        <v>152</v>
+      </c>
+      <c r="D18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" t="s">
+        <v>153</v>
+      </c>
+      <c r="D19" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C20" t="s">
+        <v>154</v>
+      </c>
+      <c r="D20" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" t="s">
+        <v>175</v>
+      </c>
+      <c r="D22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" t="s">
+        <v>149</v>
+      </c>
+      <c r="D24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" t="s">
+        <v>155</v>
+      </c>
+      <c r="D25" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" t="s">
+        <v>103</v>
+      </c>
+      <c r="C26" t="s">
+        <v>156</v>
+      </c>
+      <c r="D26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" t="s">
+        <v>104</v>
+      </c>
+      <c r="C27" t="s">
+        <v>157</v>
+      </c>
+      <c r="D27" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" t="s">
+        <v>105</v>
+      </c>
+      <c r="C28" t="s">
+        <v>158</v>
+      </c>
+      <c r="D28" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>59</v>
+      </c>
+      <c r="B29" t="s">
+        <v>106</v>
+      </c>
+      <c r="C29" t="s">
+        <v>107</v>
+      </c>
+      <c r="D29" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" t="s">
+        <v>70</v>
+      </c>
+      <c r="D30" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" t="s">
+        <v>71</v>
+      </c>
+      <c r="D31" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>69</v>
+      </c>
+      <c r="B32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" t="s">
+        <v>159</v>
+      </c>
+      <c r="D32" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>69</v>
+      </c>
+      <c r="B33" t="s">
+        <v>50</v>
+      </c>
+      <c r="C33" t="s">
+        <v>72</v>
+      </c>
+      <c r="D33" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>69</v>
+      </c>
+      <c r="B34" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" t="s">
+        <v>74</v>
+      </c>
+      <c r="D34" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>69</v>
+      </c>
+      <c r="B35" t="s">
+        <v>15</v>
+      </c>
+      <c r="C35" t="s">
+        <v>74</v>
+      </c>
+      <c r="D35" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>69</v>
+      </c>
+      <c r="B36" t="s">
+        <v>15</v>
+      </c>
+      <c r="C36" t="s">
+        <v>74</v>
+      </c>
+      <c r="D36" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>69</v>
+      </c>
+      <c r="B37" t="s">
+        <v>15</v>
+      </c>
+      <c r="C37" t="s">
+        <v>74</v>
+      </c>
+      <c r="D37" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>69</v>
+      </c>
+      <c r="B38" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" t="s">
+        <v>176</v>
+      </c>
+      <c r="D38" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>69</v>
+      </c>
+      <c r="B39" t="s">
+        <v>16</v>
+      </c>
+      <c r="C39" t="s">
+        <v>177</v>
+      </c>
+      <c r="D39" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>69</v>
+      </c>
+      <c r="B40" t="s">
+        <v>16</v>
+      </c>
+      <c r="C40" t="s">
+        <v>177</v>
+      </c>
+      <c r="D40" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>69</v>
+      </c>
+      <c r="B41" t="s">
+        <v>16</v>
+      </c>
+      <c r="C41" t="s">
+        <v>177</v>
+      </c>
+      <c r="D41" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>69</v>
+      </c>
+      <c r="B42" t="s">
+        <v>16</v>
+      </c>
+      <c r="C42" t="s">
+        <v>177</v>
+      </c>
+      <c r="D42" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>69</v>
+      </c>
+      <c r="B43" t="s">
+        <v>116</v>
+      </c>
+      <c r="C43" t="s">
+        <v>160</v>
+      </c>
+      <c r="D43" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>69</v>
+      </c>
+      <c r="B44" t="s">
+        <v>116</v>
+      </c>
+      <c r="C44" t="s">
+        <v>160</v>
+      </c>
+      <c r="D44" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>69</v>
+      </c>
+      <c r="B45" t="s">
+        <v>116</v>
+      </c>
+      <c r="C45" t="s">
+        <v>160</v>
+      </c>
+      <c r="D45" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>69</v>
+      </c>
+      <c r="B46" t="s">
+        <v>117</v>
+      </c>
+      <c r="C46" t="s">
+        <v>161</v>
+      </c>
+      <c r="D46" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>69</v>
+      </c>
+      <c r="B47" t="s">
+        <v>117</v>
+      </c>
+      <c r="C47" t="s">
+        <v>161</v>
+      </c>
+      <c r="D47" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>69</v>
+      </c>
+      <c r="B48" t="s">
+        <v>118</v>
+      </c>
+      <c r="C48" t="s">
+        <v>162</v>
+      </c>
+      <c r="D48" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>69</v>
+      </c>
+      <c r="B49" t="s">
+        <v>118</v>
+      </c>
+      <c r="C49" t="s">
+        <v>162</v>
+      </c>
+      <c r="D49" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>69</v>
+      </c>
+      <c r="B50" t="s">
+        <v>17</v>
+      </c>
+      <c r="C50" t="s">
+        <v>163</v>
+      </c>
+      <c r="D50" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>69</v>
+      </c>
+      <c r="B51" t="s">
+        <v>18</v>
+      </c>
+      <c r="C51" t="s">
+        <v>163</v>
+      </c>
+      <c r="D51" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>69</v>
+      </c>
+      <c r="B52" t="s">
+        <v>19</v>
+      </c>
+      <c r="C52" t="s">
+        <v>163</v>
+      </c>
+      <c r="D52" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>69</v>
+      </c>
+      <c r="B53" t="s">
+        <v>20</v>
+      </c>
+      <c r="C53" t="s">
+        <v>163</v>
+      </c>
+      <c r="D53" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>69</v>
+      </c>
+      <c r="B54" t="s">
+        <v>21</v>
+      </c>
+      <c r="C54" t="s">
+        <v>75</v>
+      </c>
+      <c r="D54" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>69</v>
+      </c>
+      <c r="B55" t="s">
+        <v>23</v>
+      </c>
+      <c r="C55" t="s">
+        <v>76</v>
+      </c>
+      <c r="D55" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>69</v>
+      </c>
+      <c r="B56" t="s">
+        <v>115</v>
+      </c>
+      <c r="C56" t="s">
+        <v>185</v>
+      </c>
+      <c r="D56" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>69</v>
+      </c>
+      <c r="B57" t="s">
+        <v>15</v>
+      </c>
+      <c r="C57" t="s">
+        <v>100</v>
+      </c>
+      <c r="D57" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>69</v>
+      </c>
+      <c r="B58" t="s">
+        <v>27</v>
+      </c>
+      <c r="C58" t="s">
+        <v>186</v>
+      </c>
+      <c r="D58" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>77</v>
+      </c>
+      <c r="B59" t="s">
+        <v>140</v>
+      </c>
+      <c r="C59" t="s">
+        <v>184</v>
+      </c>
+      <c r="D59" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>77</v>
+      </c>
+      <c r="B60" t="s">
+        <v>140</v>
+      </c>
+      <c r="C60" t="s">
+        <v>183</v>
+      </c>
+      <c r="D60" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>77</v>
+      </c>
+      <c r="B61" t="s">
+        <v>140</v>
+      </c>
+      <c r="C61" t="s">
+        <v>187</v>
+      </c>
+      <c r="D61" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>77</v>
+      </c>
+      <c r="B62" t="s">
+        <v>14</v>
+      </c>
+      <c r="C62" t="s">
+        <v>78</v>
+      </c>
+      <c r="D62" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>77</v>
+      </c>
+      <c r="B63" t="s">
+        <v>14</v>
+      </c>
+      <c r="C63" t="s">
+        <v>79</v>
+      </c>
+      <c r="D63" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>77</v>
+      </c>
+      <c r="B64" t="s">
+        <v>119</v>
+      </c>
+      <c r="C64" t="s">
+        <v>120</v>
+      </c>
+      <c r="D64" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>77</v>
+      </c>
+      <c r="B65" t="s">
+        <v>41</v>
+      </c>
+      <c r="C65" t="s">
+        <v>80</v>
+      </c>
+      <c r="D65" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>77</v>
+      </c>
+      <c r="B66" t="s">
+        <v>42</v>
+      </c>
+      <c r="C66" t="s">
+        <v>81</v>
+      </c>
+      <c r="D66" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>77</v>
+      </c>
+      <c r="B67" t="s">
+        <v>42</v>
+      </c>
+      <c r="C67" t="s">
+        <v>82</v>
+      </c>
+      <c r="D67" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>77</v>
+      </c>
+      <c r="B68" t="s">
+        <v>42</v>
+      </c>
+      <c r="C68" t="s">
+        <v>178</v>
+      </c>
+      <c r="D68" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>77</v>
+      </c>
+      <c r="B69" t="s">
+        <v>43</v>
+      </c>
+      <c r="C69" t="s">
+        <v>83</v>
+      </c>
+      <c r="D69" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>77</v>
+      </c>
+      <c r="B70" t="s">
+        <v>15</v>
+      </c>
+      <c r="C70" t="s">
+        <v>84</v>
+      </c>
+      <c r="D70" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>77</v>
+      </c>
+      <c r="B71" t="s">
+        <v>15</v>
+      </c>
+      <c r="C71" t="s">
+        <v>85</v>
+      </c>
+      <c r="D71" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>77</v>
+      </c>
+      <c r="B72" t="s">
+        <v>15</v>
+      </c>
+      <c r="C72" t="s">
+        <v>86</v>
+      </c>
+      <c r="D72" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>77</v>
+      </c>
+      <c r="B73" t="s">
+        <v>39</v>
+      </c>
+      <c r="C73" t="s">
+        <v>127</v>
+      </c>
+      <c r="D73" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>77</v>
+      </c>
+      <c r="B74" t="s">
+        <v>15</v>
+      </c>
+      <c r="C74" t="s">
+        <v>87</v>
+      </c>
+      <c r="D74" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>77</v>
+      </c>
+      <c r="B75" t="s">
+        <v>14</v>
+      </c>
+      <c r="C75" t="s">
+        <v>88</v>
+      </c>
+      <c r="D75" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>77</v>
+      </c>
+      <c r="B76" t="s">
+        <v>37</v>
+      </c>
+      <c r="C76" t="s">
+        <v>89</v>
+      </c>
+      <c r="D76" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>77</v>
+      </c>
+      <c r="B77" t="s">
+        <v>126</v>
+      </c>
+      <c r="C77" t="s">
+        <v>164</v>
+      </c>
+      <c r="D77" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>77</v>
+      </c>
+      <c r="B78" t="s">
+        <v>15</v>
+      </c>
+      <c r="C78" t="s">
+        <v>165</v>
+      </c>
+      <c r="D78" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>77</v>
+      </c>
+      <c r="B79" t="s">
+        <v>15</v>
+      </c>
+      <c r="C79" t="s">
+        <v>165</v>
+      </c>
+      <c r="D79" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>77</v>
+      </c>
+      <c r="B80" t="s">
+        <v>15</v>
+      </c>
+      <c r="C80" t="s">
+        <v>165</v>
+      </c>
+      <c r="D80" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>77</v>
+      </c>
+      <c r="B81" t="s">
+        <v>121</v>
+      </c>
+      <c r="C81" t="s">
+        <v>179</v>
+      </c>
+      <c r="D81" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>77</v>
+      </c>
+      <c r="B82" t="s">
+        <v>121</v>
+      </c>
+      <c r="C82" t="s">
+        <v>180</v>
+      </c>
+      <c r="D82" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>90</v>
+      </c>
+      <c r="B83" t="s">
+        <v>31</v>
+      </c>
+      <c r="C83" t="s">
+        <v>132</v>
+      </c>
+      <c r="D83" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>90</v>
+      </c>
+      <c r="B84" t="s">
+        <v>15</v>
+      </c>
+      <c r="C84" t="s">
+        <v>73</v>
+      </c>
+      <c r="D84" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>90</v>
+      </c>
+      <c r="B85" t="s">
+        <v>136</v>
+      </c>
+      <c r="C85" t="s">
+        <v>166</v>
+      </c>
+      <c r="D85" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>90</v>
+      </c>
+      <c r="B86" t="s">
+        <v>15</v>
+      </c>
+      <c r="C86" t="s">
+        <v>165</v>
+      </c>
+      <c r="D86" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>90</v>
+      </c>
+      <c r="B87" t="s">
+        <v>15</v>
+      </c>
+      <c r="C87" t="s">
+        <v>165</v>
+      </c>
+      <c r="D87" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>90</v>
+      </c>
+      <c r="B88" t="s">
+        <v>15</v>
+      </c>
+      <c r="C88" t="s">
+        <v>165</v>
+      </c>
+      <c r="D88" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>90</v>
+      </c>
+      <c r="B89" t="s">
+        <v>15</v>
+      </c>
+      <c r="C89" t="s">
+        <v>73</v>
+      </c>
+      <c r="D89" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>90</v>
+      </c>
+      <c r="B90" t="s">
+        <v>15</v>
+      </c>
+      <c r="C90" t="s">
+        <v>181</v>
+      </c>
+      <c r="D90" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>90</v>
+      </c>
+      <c r="B91" t="s">
+        <v>17</v>
+      </c>
+      <c r="C91" t="s">
+        <v>91</v>
+      </c>
+      <c r="D91" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>90</v>
+      </c>
+      <c r="B92" t="s">
+        <v>32</v>
+      </c>
+      <c r="C92" t="s">
+        <v>92</v>
+      </c>
+      <c r="D92" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>90</v>
+      </c>
+      <c r="B93" t="s">
+        <v>29</v>
+      </c>
+      <c r="C93" t="s">
+        <v>93</v>
+      </c>
+      <c r="D93" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>90</v>
+      </c>
+      <c r="B94" t="s">
+        <v>133</v>
+      </c>
+      <c r="C94" t="s">
+        <v>167</v>
+      </c>
+      <c r="D94" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>90</v>
+      </c>
+      <c r="B95" t="s">
+        <v>134</v>
+      </c>
+      <c r="C95" t="s">
+        <v>182</v>
+      </c>
+      <c r="D95" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>90</v>
+      </c>
+      <c r="B96" t="s">
+        <v>129</v>
+      </c>
+      <c r="C96" t="s">
+        <v>130</v>
+      </c>
+      <c r="D96" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>90</v>
+      </c>
+      <c r="B97" t="s">
+        <v>131</v>
+      </c>
+      <c r="C97" t="s">
+        <v>132</v>
+      </c>
+      <c r="D97" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>90</v>
+      </c>
+      <c r="B98" t="s">
+        <v>112</v>
+      </c>
+      <c r="C98" t="s">
+        <v>168</v>
+      </c>
+      <c r="D98" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>90</v>
+      </c>
+      <c r="B99" t="s">
+        <v>114</v>
+      </c>
+      <c r="C99" t="s">
+        <v>169</v>
+      </c>
+      <c r="D99" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>94</v>
+      </c>
+      <c r="B100" t="s">
+        <v>15</v>
+      </c>
+      <c r="C100" t="s">
+        <v>95</v>
+      </c>
+      <c r="D100" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>94</v>
+      </c>
+      <c r="B101" t="s">
+        <v>49</v>
+      </c>
+      <c r="C101" t="s">
+        <v>96</v>
+      </c>
+      <c r="D101" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>94</v>
+      </c>
+      <c r="B102" t="s">
+        <v>49</v>
+      </c>
+      <c r="C102" t="s">
+        <v>96</v>
+      </c>
+      <c r="D102" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>94</v>
+      </c>
+      <c r="B103" t="s">
+        <v>53</v>
+      </c>
+      <c r="C103" t="s">
+        <v>97</v>
+      </c>
+      <c r="D103" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>94</v>
+      </c>
+      <c r="B104" t="s">
+        <v>51</v>
+      </c>
+      <c r="C104" t="s">
+        <v>98</v>
+      </c>
+      <c r="D104" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>94</v>
+      </c>
+      <c r="B105" t="s">
+        <v>41</v>
+      </c>
+      <c r="C105" t="s">
+        <v>99</v>
+      </c>
+      <c r="D105" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>94</v>
+      </c>
+      <c r="B106" t="s">
+        <v>13</v>
+      </c>
+      <c r="C106" t="s">
+        <v>101</v>
+      </c>
+      <c r="D106" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>94</v>
+      </c>
+      <c r="B107" t="s">
+        <v>113</v>
+      </c>
+      <c r="C107" t="s">
+        <v>170</v>
+      </c>
+      <c r="D107" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>94</v>
+      </c>
+      <c r="B108" t="s">
+        <v>141</v>
+      </c>
+      <c r="C108" t="s">
+        <v>171</v>
+      </c>
+      <c r="D108" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>94</v>
+      </c>
+      <c r="B109" t="s">
+        <v>137</v>
+      </c>
+      <c r="C109" t="s">
+        <v>172</v>
+      </c>
+      <c r="D109" t="s">
+        <v>138</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B674A659-FCED-4227-A742-ED554B3F0E6B}">
   <dimension ref="A1:D107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -2493,12 +4052,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="139fca70-673f-44e1-94c2-b523bb9c108c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7eaf932d-7370-48c5-9459-ae540daf9d7d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2709,20 +4270,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="139fca70-673f-44e1-94c2-b523bb9c108c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7eaf932d-7370-48c5-9459-ae540daf9d7d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BB2BB8B-BA4E-4835-AC34-431A62162A7D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B57CF69-5D19-450C-935B-68EC43A8DA31}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="139fca70-673f-44e1-94c2-b523bb9c108c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="7eaf932d-7370-48c5-9459-ae540daf9d7d"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2747,18 +4315,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B57CF69-5D19-450C-935B-68EC43A8DA31}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BB2BB8B-BA4E-4835-AC34-431A62162A7D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="139fca70-673f-44e1-94c2-b523bb9c108c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="7eaf932d-7370-48c5-9459-ae540daf9d7d"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Implement process search functionality in Process Flow view
- Added a search input for users to find specific processes within the Process Flow view.
- Implemented search logic to filter processes based on user input, displaying results dynamically.
- Enhanced navigation to specific process nodes upon selection from search results.
- Updated the initialization of search functionality to ensure it is set up after rendering the process flow.
- Removed zoom in/out buttons to streamline the interface and focus on search capabilities.
</commit_message>
<xml_diff>
--- a/Connections.xlsx
+++ b/Connections.xlsx
@@ -8,17 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eyus-my.sharepoint.com/personal/tony_calabro_ey_com/Documents/Desktop/Cursor/Hierarchy 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="8_{A326F537-9C9C-4DE6-A793-9A61B1FAA38A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC3E6FF6-3F2F-41B7-8AE7-37F1CEC831BF}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="8_{A326F537-9C9C-4DE6-A793-9A61B1FAA38A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1DFD12A1-980A-46DD-95EA-8A1B8C87BE17}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C5CF7D8D-18C1-4DA6-BBC5-CBC3C1BDFBAD}"/>
   </bookViews>
   <sheets>
-    <sheet name="Connections" sheetId="7" r:id="rId1"/>
-    <sheet name="Previous Update v4" sheetId="8" r:id="rId2"/>
+    <sheet name="Connections" sheetId="9" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Connections!$A$1:$D$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Previous Update v4'!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -41,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="189">
   <si>
     <t>Plan and Procure Metering Assets</t>
   </si>
@@ -334,12 +332,6 @@
     <t>Data Lake Record</t>
   </si>
   <si>
-    <t>Reference Information</t>
-  </si>
-  <si>
-    <t>Security Policy / Access Control</t>
-  </si>
-  <si>
     <t>Investigation Case</t>
   </si>
   <si>
@@ -559,9 +551,6 @@
     <t>Cross-System Anomaly</t>
   </si>
   <si>
-    <t>DI App / Edge Model</t>
-  </si>
-  <si>
     <t>Configuration Prerequisite</t>
   </si>
   <si>
@@ -605,6 +594,18 @@
   </si>
   <si>
     <t>Grid Asset Alarm</t>
+  </si>
+  <si>
+    <t>Data Exception</t>
+  </si>
+  <si>
+    <t>Customer Usage View</t>
+  </si>
+  <si>
+    <t>Service Escalation</t>
+  </si>
+  <si>
+    <t>DI Data Schema</t>
   </si>
 </sst>
 </file>
@@ -984,11 +985,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16457C1E-DB35-46F2-9BC1-E2CF8C3A2E02}">
-  <dimension ref="A1:D109"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4C1D8E9-FEAA-4032-8F7B-225924646E77}">
+  <dimension ref="A1:D113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:XFD24"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="B108" sqref="B108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1035,10 +1036,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1046,10 +1047,10 @@
         <v>59</v>
       </c>
       <c r="B4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D4" t="s">
         <v>2</v>
@@ -1105,7 +1106,7 @@
         <v>48</v>
       </c>
       <c r="C8" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D8" t="s">
         <v>54</v>
@@ -1161,10 +1162,10 @@
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D12" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1175,7 +1176,7 @@
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D13" t="s">
         <v>6</v>
@@ -1186,10 +1187,10 @@
         <v>59</v>
       </c>
       <c r="B14" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C14" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D14" t="s">
         <v>54</v>
@@ -1200,13 +1201,13 @@
         <v>59</v>
       </c>
       <c r="B15" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D15" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1214,10 +1215,10 @@
         <v>59</v>
       </c>
       <c r="B16" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C16" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D16" t="s">
         <v>7</v>
@@ -1228,13 +1229,13 @@
         <v>59</v>
       </c>
       <c r="B17" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C17" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D17" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1245,7 +1246,7 @@
         <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D18" t="s">
         <v>7</v>
@@ -1259,10 +1260,10 @@
         <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D19" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1270,13 +1271,13 @@
         <v>59</v>
       </c>
       <c r="B20" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C20" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D20" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1301,7 +1302,7 @@
         <v>7</v>
       </c>
       <c r="C22" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D22" t="s">
         <v>14</v>
@@ -1329,7 +1330,7 @@
         <v>9</v>
       </c>
       <c r="C24" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D24" t="s">
         <v>7</v>
@@ -1343,10 +1344,10 @@
         <v>6</v>
       </c>
       <c r="C25" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D25" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1354,10 +1355,10 @@
         <v>59</v>
       </c>
       <c r="B26" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C26" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D26" t="s">
         <v>3</v>
@@ -1368,13 +1369,13 @@
         <v>59</v>
       </c>
       <c r="B27" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C27" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D27" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1382,13 +1383,13 @@
         <v>59</v>
       </c>
       <c r="B28" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C28" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D28" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1396,10 +1397,10 @@
         <v>59</v>
       </c>
       <c r="B29" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C29" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D29" t="s">
         <v>54</v>
@@ -1441,10 +1442,10 @@
         <v>14</v>
       </c>
       <c r="C32" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D32" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1525,7 +1526,7 @@
         <v>15</v>
       </c>
       <c r="C38" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D38" t="s">
         <v>16</v>
@@ -1536,13 +1537,13 @@
         <v>69</v>
       </c>
       <c r="B39" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C39" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="D39" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1553,10 +1554,10 @@
         <v>16</v>
       </c>
       <c r="C40" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D40" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1567,10 +1568,10 @@
         <v>16</v>
       </c>
       <c r="C41" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D41" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1581,10 +1582,10 @@
         <v>16</v>
       </c>
       <c r="C42" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D42" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1592,13 +1593,13 @@
         <v>69</v>
       </c>
       <c r="B43" t="s">
-        <v>116</v>
+        <v>16</v>
       </c>
       <c r="C43" t="s">
-        <v>160</v>
+        <v>174</v>
       </c>
       <c r="D43" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1606,13 +1607,13 @@
         <v>69</v>
       </c>
       <c r="B44" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C44" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D44" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1620,13 +1621,13 @@
         <v>69</v>
       </c>
       <c r="B45" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C45" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D45" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1634,13 +1635,13 @@
         <v>69</v>
       </c>
       <c r="B46" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C46" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D46" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1648,13 +1649,13 @@
         <v>69</v>
       </c>
       <c r="B47" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C47" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D47" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1662,13 +1663,13 @@
         <v>69</v>
       </c>
       <c r="B48" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C48" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D48" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1676,13 +1677,13 @@
         <v>69</v>
       </c>
       <c r="B49" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C49" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D49" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1690,13 +1691,13 @@
         <v>69</v>
       </c>
       <c r="B50" t="s">
-        <v>17</v>
+        <v>116</v>
       </c>
       <c r="C50" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D50" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1704,10 +1705,10 @@
         <v>69</v>
       </c>
       <c r="B51" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C51" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D51" t="s">
         <v>21</v>
@@ -1718,10 +1719,10 @@
         <v>69</v>
       </c>
       <c r="B52" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C52" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D52" t="s">
         <v>21</v>
@@ -1732,10 +1733,10 @@
         <v>69</v>
       </c>
       <c r="B53" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C53" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D53" t="s">
         <v>21</v>
@@ -1746,13 +1747,13 @@
         <v>69</v>
       </c>
       <c r="B54" t="s">
+        <v>20</v>
+      </c>
+      <c r="C54" t="s">
+        <v>161</v>
+      </c>
+      <c r="D54" t="s">
         <v>21</v>
-      </c>
-      <c r="C54" t="s">
-        <v>75</v>
-      </c>
-      <c r="D54" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1760,13 +1761,13 @@
         <v>69</v>
       </c>
       <c r="B55" t="s">
+        <v>21</v>
+      </c>
+      <c r="C55" t="s">
+        <v>75</v>
+      </c>
+      <c r="D55" t="s">
         <v>23</v>
-      </c>
-      <c r="C55" t="s">
-        <v>76</v>
-      </c>
-      <c r="D55" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -1774,13 +1775,13 @@
         <v>69</v>
       </c>
       <c r="B56" t="s">
-        <v>115</v>
+        <v>23</v>
       </c>
       <c r="C56" t="s">
-        <v>185</v>
+        <v>76</v>
       </c>
       <c r="D56" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -1788,10 +1789,10 @@
         <v>69</v>
       </c>
       <c r="B57" t="s">
-        <v>15</v>
+        <v>113</v>
       </c>
       <c r="C57" t="s">
-        <v>100</v>
+        <v>182</v>
       </c>
       <c r="D57" t="s">
         <v>27</v>
@@ -1802,27 +1803,27 @@
         <v>69</v>
       </c>
       <c r="B58" t="s">
+        <v>15</v>
+      </c>
+      <c r="C58" t="s">
+        <v>98</v>
+      </c>
+      <c r="D58" t="s">
         <v>27</v>
-      </c>
-      <c r="C58" t="s">
-        <v>186</v>
-      </c>
-      <c r="D58" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="B59" t="s">
-        <v>140</v>
+        <v>27</v>
       </c>
       <c r="C59" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D59" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -1830,13 +1831,13 @@
         <v>77</v>
       </c>
       <c r="B60" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C60" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D60" t="s">
-        <v>141</v>
+        <v>27</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -1844,13 +1845,13 @@
         <v>77</v>
       </c>
       <c r="B61" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C61" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="D61" t="s">
-        <v>11</v>
+        <v>139</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -1858,13 +1859,13 @@
         <v>77</v>
       </c>
       <c r="B62" t="s">
-        <v>14</v>
+        <v>138</v>
       </c>
       <c r="C62" t="s">
-        <v>78</v>
+        <v>184</v>
       </c>
       <c r="D62" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -1875,10 +1876,10 @@
         <v>14</v>
       </c>
       <c r="C63" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D63" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -1886,10 +1887,10 @@
         <v>77</v>
       </c>
       <c r="B64" t="s">
-        <v>119</v>
+        <v>14</v>
       </c>
       <c r="C64" t="s">
-        <v>120</v>
+        <v>79</v>
       </c>
       <c r="D64" t="s">
         <v>41</v>
@@ -1900,13 +1901,13 @@
         <v>77</v>
       </c>
       <c r="B65" t="s">
+        <v>117</v>
+      </c>
+      <c r="C65" t="s">
+        <v>118</v>
+      </c>
+      <c r="D65" t="s">
         <v>41</v>
-      </c>
-      <c r="C65" t="s">
-        <v>80</v>
-      </c>
-      <c r="D65" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -1914,13 +1915,13 @@
         <v>77</v>
       </c>
       <c r="B66" t="s">
+        <v>41</v>
+      </c>
+      <c r="C66" t="s">
+        <v>80</v>
+      </c>
+      <c r="D66" t="s">
         <v>42</v>
-      </c>
-      <c r="C66" t="s">
-        <v>81</v>
-      </c>
-      <c r="D66" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -1931,10 +1932,10 @@
         <v>42</v>
       </c>
       <c r="C67" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D67" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -1945,10 +1946,10 @@
         <v>42</v>
       </c>
       <c r="C68" t="s">
-        <v>178</v>
+        <v>82</v>
       </c>
       <c r="D68" t="s">
-        <v>141</v>
+        <v>43</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -1956,13 +1957,13 @@
         <v>77</v>
       </c>
       <c r="B69" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C69" t="s">
-        <v>83</v>
+        <v>175</v>
       </c>
       <c r="D69" t="s">
-        <v>44</v>
+        <v>139</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -1970,13 +1971,13 @@
         <v>77</v>
       </c>
       <c r="B70" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="C70" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D70" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -1987,10 +1988,10 @@
         <v>15</v>
       </c>
       <c r="C71" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D71" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -2001,10 +2002,10 @@
         <v>15</v>
       </c>
       <c r="C72" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D72" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -2012,13 +2013,13 @@
         <v>77</v>
       </c>
       <c r="B73" t="s">
+        <v>15</v>
+      </c>
+      <c r="C73" t="s">
+        <v>86</v>
+      </c>
+      <c r="D73" t="s">
         <v>39</v>
-      </c>
-      <c r="C73" t="s">
-        <v>127</v>
-      </c>
-      <c r="D73" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -2026,13 +2027,13 @@
         <v>77</v>
       </c>
       <c r="B74" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="C74" t="s">
-        <v>87</v>
+        <v>125</v>
       </c>
       <c r="D74" t="s">
-        <v>35</v>
+        <v>126</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -2040,13 +2041,13 @@
         <v>77</v>
       </c>
       <c r="B75" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C75" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D75" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -2054,13 +2055,13 @@
         <v>77</v>
       </c>
       <c r="B76" t="s">
+        <v>14</v>
+      </c>
+      <c r="C76" t="s">
+        <v>88</v>
+      </c>
+      <c r="D76" t="s">
         <v>37</v>
-      </c>
-      <c r="C76" t="s">
-        <v>89</v>
-      </c>
-      <c r="D76" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -2068,13 +2069,13 @@
         <v>77</v>
       </c>
       <c r="B77" t="s">
-        <v>126</v>
+        <v>37</v>
       </c>
       <c r="C77" t="s">
-        <v>164</v>
+        <v>89</v>
       </c>
       <c r="D77" t="s">
-        <v>113</v>
+        <v>38</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -2082,13 +2083,13 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>15</v>
+        <v>124</v>
       </c>
       <c r="C78" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D78" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -2099,10 +2100,10 @@
         <v>15</v>
       </c>
       <c r="C79" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D79" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -2113,10 +2114,10 @@
         <v>15</v>
       </c>
       <c r="C80" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D80" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -2124,13 +2125,13 @@
         <v>77</v>
       </c>
       <c r="B81" t="s">
-        <v>121</v>
+        <v>15</v>
       </c>
       <c r="C81" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
       <c r="D81" t="s">
-        <v>11</v>
+        <v>123</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -2138,27 +2139,27 @@
         <v>77</v>
       </c>
       <c r="B82" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C82" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D82" t="s">
-        <v>122</v>
+        <v>11</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="B83" t="s">
-        <v>31</v>
+        <v>119</v>
       </c>
       <c r="C83" t="s">
-        <v>132</v>
+        <v>177</v>
       </c>
       <c r="D83" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -2166,13 +2167,13 @@
         <v>90</v>
       </c>
       <c r="B84" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="C84" t="s">
-        <v>73</v>
+        <v>130</v>
       </c>
       <c r="D84" t="s">
-        <v>32</v>
+        <v>106</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -2180,10 +2181,10 @@
         <v>90</v>
       </c>
       <c r="B85" t="s">
-        <v>136</v>
+        <v>15</v>
       </c>
       <c r="C85" t="s">
-        <v>166</v>
+        <v>73</v>
       </c>
       <c r="D85" t="s">
         <v>32</v>
@@ -2194,13 +2195,13 @@
         <v>90</v>
       </c>
       <c r="B86" t="s">
-        <v>15</v>
+        <v>134</v>
       </c>
       <c r="C86" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D86" t="s">
-        <v>136</v>
+        <v>32</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -2211,10 +2212,10 @@
         <v>15</v>
       </c>
       <c r="C87" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D87" t="s">
-        <v>115</v>
+        <v>134</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -2225,10 +2226,10 @@
         <v>15</v>
       </c>
       <c r="C88" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D88" t="s">
-        <v>135</v>
+        <v>113</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -2239,10 +2240,10 @@
         <v>15</v>
       </c>
       <c r="C89" t="s">
-        <v>73</v>
+        <v>163</v>
       </c>
       <c r="D89" t="s">
-        <v>34</v>
+        <v>133</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -2253,10 +2254,10 @@
         <v>15</v>
       </c>
       <c r="C90" t="s">
-        <v>181</v>
+        <v>73</v>
       </c>
       <c r="D90" t="s">
-        <v>143</v>
+        <v>34</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -2264,13 +2265,13 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C91" t="s">
-        <v>91</v>
+        <v>178</v>
       </c>
       <c r="D91" t="s">
-        <v>34</v>
+        <v>141</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -2278,13 +2279,13 @@
         <v>90</v>
       </c>
       <c r="B92" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="C92" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D92" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -2292,13 +2293,13 @@
         <v>90</v>
       </c>
       <c r="B93" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C93" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D93" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -2306,13 +2307,13 @@
         <v>90</v>
       </c>
       <c r="B94" t="s">
-        <v>133</v>
+        <v>32</v>
       </c>
       <c r="C94" t="s">
-        <v>167</v>
+        <v>186</v>
       </c>
       <c r="D94" t="s">
-        <v>134</v>
+        <v>25</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -2320,13 +2321,13 @@
         <v>90</v>
       </c>
       <c r="B95" t="s">
-        <v>134</v>
+        <v>25</v>
       </c>
       <c r="C95" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="D95" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -2334,13 +2335,13 @@
         <v>90</v>
       </c>
       <c r="B96" t="s">
-        <v>129</v>
+        <v>25</v>
       </c>
       <c r="C96" t="s">
-        <v>130</v>
+        <v>93</v>
       </c>
       <c r="D96" t="s">
-        <v>113</v>
+        <v>29</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -2348,13 +2349,13 @@
         <v>90</v>
       </c>
       <c r="B97" t="s">
-        <v>131</v>
+        <v>29</v>
       </c>
       <c r="C97" t="s">
-        <v>132</v>
+        <v>93</v>
       </c>
       <c r="D97" t="s">
-        <v>113</v>
+        <v>30</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -2362,13 +2363,13 @@
         <v>90</v>
       </c>
       <c r="B98" t="s">
-        <v>112</v>
+        <v>131</v>
       </c>
       <c r="C98" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D98" t="s">
-        <v>113</v>
+        <v>132</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -2376,69 +2377,69 @@
         <v>90</v>
       </c>
       <c r="B99" t="s">
-        <v>114</v>
+        <v>132</v>
       </c>
       <c r="C99" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="D99" t="s">
-        <v>113</v>
+        <v>14</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B100" t="s">
-        <v>15</v>
+        <v>127</v>
       </c>
       <c r="C100" t="s">
-        <v>95</v>
+        <v>128</v>
       </c>
       <c r="D100" t="s">
-        <v>49</v>
+        <v>111</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B101" t="s">
-        <v>49</v>
+        <v>129</v>
       </c>
       <c r="C101" t="s">
-        <v>96</v>
+        <v>130</v>
       </c>
       <c r="D101" t="s">
-        <v>52</v>
+        <v>111</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B102" t="s">
-        <v>49</v>
+        <v>110</v>
       </c>
       <c r="C102" t="s">
-        <v>96</v>
+        <v>166</v>
       </c>
       <c r="D102" t="s">
-        <v>53</v>
+        <v>111</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B103" t="s">
-        <v>53</v>
+        <v>112</v>
       </c>
       <c r="C103" t="s">
-        <v>97</v>
+        <v>167</v>
       </c>
       <c r="D103" t="s">
-        <v>25</v>
+        <v>111</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -2446,13 +2447,13 @@
         <v>94</v>
       </c>
       <c r="B104" t="s">
-        <v>51</v>
+        <v>15</v>
       </c>
       <c r="C104" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D104" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -2460,13 +2461,13 @@
         <v>94</v>
       </c>
       <c r="B105" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="C105" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D105" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -2474,13 +2475,13 @@
         <v>94</v>
       </c>
       <c r="B106" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="C106" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D106" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -2488,13 +2489,7 @@
         <v>94</v>
       </c>
       <c r="B107" t="s">
-        <v>113</v>
-      </c>
-      <c r="C107" t="s">
-        <v>170</v>
-      </c>
-      <c r="D107" t="s">
-        <v>139</v>
+        <v>51</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -2502,13 +2497,13 @@
         <v>94</v>
       </c>
       <c r="B108" t="s">
-        <v>141</v>
+        <v>41</v>
       </c>
       <c r="C108" t="s">
-        <v>171</v>
+        <v>97</v>
       </c>
       <c r="D108" t="s">
-        <v>142</v>
+        <v>11</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -2516,1533 +2511,63 @@
         <v>94</v>
       </c>
       <c r="B109" t="s">
+        <v>13</v>
+      </c>
+      <c r="C109" t="s">
+        <v>99</v>
+      </c>
+      <c r="D109" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>94</v>
+      </c>
+      <c r="B110" t="s">
+        <v>111</v>
+      </c>
+      <c r="C110" t="s">
+        <v>168</v>
+      </c>
+      <c r="D110" t="s">
         <v>137</v>
       </c>
-      <c r="C109" t="s">
-        <v>172</v>
-      </c>
-      <c r="D109" t="s">
-        <v>138</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B674A659-FCED-4227-A742-ED554B3F0E6B}">
-  <dimension ref="A1:D107"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="39.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="59.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="59.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>144</v>
-      </c>
-      <c r="D3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B4" t="s">
-        <v>102</v>
-      </c>
-      <c r="C4" t="s">
-        <v>145</v>
-      </c>
-      <c r="D4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" t="s">
-        <v>63</v>
-      </c>
-      <c r="D6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>59</v>
-      </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>59</v>
-      </c>
-      <c r="B8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8" t="s">
-        <v>173</v>
-      </c>
-      <c r="D8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>59</v>
-      </c>
-      <c r="B9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" t="s">
-        <v>64</v>
-      </c>
-      <c r="D9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>59</v>
-      </c>
-      <c r="B10" t="s">
-        <v>54</v>
-      </c>
-      <c r="C10" t="s">
-        <v>65</v>
-      </c>
-      <c r="D10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>59</v>
-      </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" t="s">
-        <v>66</v>
-      </c>
-      <c r="D11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>59</v>
-      </c>
-      <c r="B12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" t="s">
-        <v>146</v>
-      </c>
-      <c r="D12" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>59</v>
-      </c>
-      <c r="B13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" t="s">
-        <v>174</v>
-      </c>
-      <c r="D13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>59</v>
-      </c>
-      <c r="B14" t="s">
-        <v>109</v>
-      </c>
-      <c r="C14" t="s">
-        <v>147</v>
-      </c>
-      <c r="D14" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>59</v>
-      </c>
-      <c r="B15" t="s">
-        <v>109</v>
-      </c>
-      <c r="C15" t="s">
-        <v>148</v>
-      </c>
-      <c r="D15" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>59</v>
-      </c>
-      <c r="B16" t="s">
-        <v>108</v>
-      </c>
-      <c r="C16" t="s">
-        <v>149</v>
-      </c>
-      <c r="D16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>59</v>
-      </c>
-      <c r="B17" t="s">
-        <v>108</v>
-      </c>
-      <c r="C17" t="s">
-        <v>150</v>
-      </c>
-      <c r="D17" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>59</v>
-      </c>
-      <c r="B18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" t="s">
-        <v>152</v>
-      </c>
-      <c r="D18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>59</v>
-      </c>
-      <c r="B19" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" t="s">
-        <v>153</v>
-      </c>
-      <c r="D19" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>59</v>
-      </c>
-      <c r="B20" t="s">
-        <v>111</v>
-      </c>
-      <c r="C20" t="s">
-        <v>154</v>
-      </c>
-      <c r="D20" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>59</v>
-      </c>
-      <c r="B21" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" t="s">
-        <v>68</v>
-      </c>
-      <c r="D21" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>59</v>
-      </c>
-      <c r="B22" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" t="s">
-        <v>175</v>
-      </c>
-      <c r="D22" t="s">
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>94</v>
+      </c>
+      <c r="B111" t="s">
+        <v>139</v>
+      </c>
+      <c r="C111" t="s">
+        <v>169</v>
+      </c>
+      <c r="D111" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>94</v>
+      </c>
+      <c r="B112" t="s">
+        <v>135</v>
+      </c>
+      <c r="C112" t="s">
+        <v>188</v>
+      </c>
+      <c r="D112" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>59</v>
-      </c>
-      <c r="B23" t="s">
-        <v>47</v>
-      </c>
-      <c r="C23" t="s">
-        <v>67</v>
-      </c>
-      <c r="D23" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>59</v>
-      </c>
-      <c r="B24" t="s">
-        <v>9</v>
-      </c>
-      <c r="C24" t="s">
-        <v>149</v>
-      </c>
-      <c r="D24" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>59</v>
-      </c>
-      <c r="B25" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" t="s">
-        <v>155</v>
-      </c>
-      <c r="D25" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>59</v>
-      </c>
-      <c r="B26" t="s">
-        <v>103</v>
-      </c>
-      <c r="C26" t="s">
-        <v>156</v>
-      </c>
-      <c r="D26" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>59</v>
-      </c>
-      <c r="B27" t="s">
-        <v>104</v>
-      </c>
-      <c r="C27" t="s">
-        <v>157</v>
-      </c>
-      <c r="D27" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>59</v>
-      </c>
-      <c r="B28" t="s">
-        <v>105</v>
-      </c>
-      <c r="C28" t="s">
-        <v>158</v>
-      </c>
-      <c r="D28" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>59</v>
-      </c>
-      <c r="B29" t="s">
-        <v>106</v>
-      </c>
-      <c r="C29" t="s">
-        <v>107</v>
-      </c>
-      <c r="D29" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>69</v>
-      </c>
-      <c r="B30" t="s">
-        <v>46</v>
-      </c>
-      <c r="C30" t="s">
-        <v>70</v>
-      </c>
-      <c r="D30" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>69</v>
-      </c>
-      <c r="B31" t="s">
-        <v>14</v>
-      </c>
-      <c r="C31" t="s">
-        <v>71</v>
-      </c>
-      <c r="D31" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>69</v>
-      </c>
-      <c r="B32" t="s">
-        <v>14</v>
-      </c>
-      <c r="C32" t="s">
-        <v>159</v>
-      </c>
-      <c r="D32" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>69</v>
-      </c>
-      <c r="B33" t="s">
-        <v>50</v>
-      </c>
-      <c r="C33" t="s">
-        <v>72</v>
-      </c>
-      <c r="D33" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>69</v>
-      </c>
-      <c r="B34" t="s">
-        <v>15</v>
-      </c>
-      <c r="C34" t="s">
-        <v>74</v>
-      </c>
-      <c r="D34" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>69</v>
-      </c>
-      <c r="B35" t="s">
-        <v>15</v>
-      </c>
-      <c r="C35" t="s">
-        <v>74</v>
-      </c>
-      <c r="D35" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>69</v>
-      </c>
-      <c r="B36" t="s">
-        <v>15</v>
-      </c>
-      <c r="C36" t="s">
-        <v>74</v>
-      </c>
-      <c r="D36" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>69</v>
-      </c>
-      <c r="B37" t="s">
-        <v>15</v>
-      </c>
-      <c r="C37" t="s">
-        <v>74</v>
-      </c>
-      <c r="D37" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>69</v>
-      </c>
-      <c r="B38" t="s">
-        <v>15</v>
-      </c>
-      <c r="C38" t="s">
-        <v>176</v>
-      </c>
-      <c r="D38" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>69</v>
-      </c>
-      <c r="B39" t="s">
-        <v>16</v>
-      </c>
-      <c r="C39" t="s">
-        <v>177</v>
-      </c>
-      <c r="D39" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>69</v>
-      </c>
-      <c r="B40" t="s">
-        <v>16</v>
-      </c>
-      <c r="C40" t="s">
-        <v>177</v>
-      </c>
-      <c r="D40" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>69</v>
-      </c>
-      <c r="B41" t="s">
-        <v>16</v>
-      </c>
-      <c r="C41" t="s">
-        <v>177</v>
-      </c>
-      <c r="D41" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>69</v>
-      </c>
-      <c r="B42" t="s">
-        <v>16</v>
-      </c>
-      <c r="C42" t="s">
-        <v>177</v>
-      </c>
-      <c r="D42" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>69</v>
-      </c>
-      <c r="B43" t="s">
-        <v>116</v>
-      </c>
-      <c r="C43" t="s">
-        <v>160</v>
-      </c>
-      <c r="D43" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>69</v>
-      </c>
-      <c r="B44" t="s">
-        <v>116</v>
-      </c>
-      <c r="C44" t="s">
-        <v>160</v>
-      </c>
-      <c r="D44" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>69</v>
-      </c>
-      <c r="B45" t="s">
-        <v>116</v>
-      </c>
-      <c r="C45" t="s">
-        <v>160</v>
-      </c>
-      <c r="D45" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>69</v>
-      </c>
-      <c r="B46" t="s">
-        <v>117</v>
-      </c>
-      <c r="C46" t="s">
-        <v>161</v>
-      </c>
-      <c r="D46" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>69</v>
-      </c>
-      <c r="B47" t="s">
-        <v>117</v>
-      </c>
-      <c r="C47" t="s">
-        <v>161</v>
-      </c>
-      <c r="D47" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>69</v>
-      </c>
-      <c r="B48" t="s">
-        <v>118</v>
-      </c>
-      <c r="C48" t="s">
-        <v>162</v>
-      </c>
-      <c r="D48" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>69</v>
-      </c>
-      <c r="B49" t="s">
-        <v>118</v>
-      </c>
-      <c r="C49" t="s">
-        <v>162</v>
-      </c>
-      <c r="D49" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>69</v>
-      </c>
-      <c r="B50" t="s">
-        <v>17</v>
-      </c>
-      <c r="C50" t="s">
-        <v>163</v>
-      </c>
-      <c r="D50" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>69</v>
-      </c>
-      <c r="B51" t="s">
-        <v>18</v>
-      </c>
-      <c r="C51" t="s">
-        <v>163</v>
-      </c>
-      <c r="D51" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>69</v>
-      </c>
-      <c r="B52" t="s">
-        <v>19</v>
-      </c>
-      <c r="C52" t="s">
-        <v>163</v>
-      </c>
-      <c r="D52" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>69</v>
-      </c>
-      <c r="B53" t="s">
-        <v>20</v>
-      </c>
-      <c r="C53" t="s">
-        <v>163</v>
-      </c>
-      <c r="D53" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>69</v>
-      </c>
-      <c r="B54" t="s">
-        <v>21</v>
-      </c>
-      <c r="C54" t="s">
-        <v>75</v>
-      </c>
-      <c r="D54" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>69</v>
-      </c>
-      <c r="B55" t="s">
-        <v>23</v>
-      </c>
-      <c r="C55" t="s">
-        <v>76</v>
-      </c>
-      <c r="D55" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>77</v>
-      </c>
-      <c r="B56" t="s">
-        <v>14</v>
-      </c>
-      <c r="C56" t="s">
-        <v>78</v>
-      </c>
-      <c r="D56" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>77</v>
-      </c>
-      <c r="B57" t="s">
-        <v>14</v>
-      </c>
-      <c r="C57" t="s">
-        <v>79</v>
-      </c>
-      <c r="D57" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>77</v>
-      </c>
-      <c r="B58" t="s">
-        <v>119</v>
-      </c>
-      <c r="C58" t="s">
-        <v>120</v>
-      </c>
-      <c r="D58" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>77</v>
-      </c>
-      <c r="B59" t="s">
-        <v>41</v>
-      </c>
-      <c r="C59" t="s">
-        <v>80</v>
-      </c>
-      <c r="D59" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>77</v>
-      </c>
-      <c r="B60" t="s">
-        <v>42</v>
-      </c>
-      <c r="C60" t="s">
-        <v>81</v>
-      </c>
-      <c r="D60" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>77</v>
-      </c>
-      <c r="B61" t="s">
-        <v>42</v>
-      </c>
-      <c r="C61" t="s">
-        <v>82</v>
-      </c>
-      <c r="D61" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>77</v>
-      </c>
-      <c r="B62" t="s">
-        <v>42</v>
-      </c>
-      <c r="C62" t="s">
-        <v>178</v>
-      </c>
-      <c r="D62" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>77</v>
-      </c>
-      <c r="B63" t="s">
-        <v>43</v>
-      </c>
-      <c r="C63" t="s">
-        <v>83</v>
-      </c>
-      <c r="D63" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>77</v>
-      </c>
-      <c r="B64" t="s">
-        <v>15</v>
-      </c>
-      <c r="C64" t="s">
-        <v>84</v>
-      </c>
-      <c r="D64" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>77</v>
-      </c>
-      <c r="B65" t="s">
-        <v>15</v>
-      </c>
-      <c r="C65" t="s">
-        <v>85</v>
-      </c>
-      <c r="D65" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>77</v>
-      </c>
-      <c r="B66" t="s">
-        <v>15</v>
-      </c>
-      <c r="C66" t="s">
-        <v>86</v>
-      </c>
-      <c r="D66" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>77</v>
-      </c>
-      <c r="B67" t="s">
-        <v>39</v>
-      </c>
-      <c r="C67" t="s">
-        <v>127</v>
-      </c>
-      <c r="D67" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>77</v>
-      </c>
-      <c r="B68" t="s">
-        <v>15</v>
-      </c>
-      <c r="C68" t="s">
-        <v>87</v>
-      </c>
-      <c r="D68" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>77</v>
-      </c>
-      <c r="B69" t="s">
-        <v>14</v>
-      </c>
-      <c r="C69" t="s">
-        <v>88</v>
-      </c>
-      <c r="D69" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>77</v>
-      </c>
-      <c r="B70" t="s">
-        <v>37</v>
-      </c>
-      <c r="C70" t="s">
-        <v>89</v>
-      </c>
-      <c r="D70" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>77</v>
-      </c>
-      <c r="B71" t="s">
-        <v>126</v>
-      </c>
-      <c r="C71" t="s">
-        <v>164</v>
-      </c>
-      <c r="D71" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>77</v>
-      </c>
-      <c r="B72" t="s">
-        <v>15</v>
-      </c>
-      <c r="C72" t="s">
-        <v>165</v>
-      </c>
-      <c r="D72" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>77</v>
-      </c>
-      <c r="B73" t="s">
-        <v>15</v>
-      </c>
-      <c r="C73" t="s">
-        <v>165</v>
-      </c>
-      <c r="D73" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>77</v>
-      </c>
-      <c r="B74" t="s">
-        <v>15</v>
-      </c>
-      <c r="C74" t="s">
-        <v>165</v>
-      </c>
-      <c r="D74" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>77</v>
-      </c>
-      <c r="B75" t="s">
-        <v>121</v>
-      </c>
-      <c r="C75" t="s">
-        <v>179</v>
-      </c>
-      <c r="D75" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>77</v>
-      </c>
-      <c r="B76" t="s">
-        <v>121</v>
-      </c>
-      <c r="C76" t="s">
-        <v>180</v>
-      </c>
-      <c r="D76" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>90</v>
-      </c>
-      <c r="B77" t="s">
-        <v>31</v>
-      </c>
-      <c r="C77" t="s">
-        <v>132</v>
-      </c>
-      <c r="D77" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>90</v>
-      </c>
-      <c r="B78" t="s">
-        <v>15</v>
-      </c>
-      <c r="C78" t="s">
-        <v>73</v>
-      </c>
-      <c r="D78" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>90</v>
-      </c>
-      <c r="B79" t="s">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>94</v>
+      </c>
+      <c r="B113" t="s">
         <v>136</v>
-      </c>
-      <c r="C79" t="s">
-        <v>166</v>
-      </c>
-      <c r="D79" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>90</v>
-      </c>
-      <c r="B80" t="s">
-        <v>15</v>
-      </c>
-      <c r="C80" t="s">
-        <v>165</v>
-      </c>
-      <c r="D80" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>90</v>
-      </c>
-      <c r="B81" t="s">
-        <v>15</v>
-      </c>
-      <c r="C81" t="s">
-        <v>165</v>
-      </c>
-      <c r="D81" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>90</v>
-      </c>
-      <c r="B82" t="s">
-        <v>15</v>
-      </c>
-      <c r="C82" t="s">
-        <v>165</v>
-      </c>
-      <c r="D82" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>90</v>
-      </c>
-      <c r="B83" t="s">
-        <v>15</v>
-      </c>
-      <c r="C83" t="s">
-        <v>73</v>
-      </c>
-      <c r="D83" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>90</v>
-      </c>
-      <c r="B84" t="s">
-        <v>15</v>
-      </c>
-      <c r="C84" t="s">
-        <v>181</v>
-      </c>
-      <c r="D84" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>90</v>
-      </c>
-      <c r="B85" t="s">
-        <v>17</v>
-      </c>
-      <c r="C85" t="s">
-        <v>91</v>
-      </c>
-      <c r="D85" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>90</v>
-      </c>
-      <c r="B86" t="s">
-        <v>32</v>
-      </c>
-      <c r="C86" t="s">
-        <v>92</v>
-      </c>
-      <c r="D86" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>90</v>
-      </c>
-      <c r="B87" t="s">
-        <v>29</v>
-      </c>
-      <c r="C87" t="s">
-        <v>93</v>
-      </c>
-      <c r="D87" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>90</v>
-      </c>
-      <c r="B88" t="s">
-        <v>133</v>
-      </c>
-      <c r="C88" t="s">
-        <v>167</v>
-      </c>
-      <c r="D88" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>90</v>
-      </c>
-      <c r="B89" t="s">
-        <v>134</v>
-      </c>
-      <c r="C89" t="s">
-        <v>182</v>
-      </c>
-      <c r="D89" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>90</v>
-      </c>
-      <c r="B90" t="s">
-        <v>129</v>
-      </c>
-      <c r="C90" t="s">
-        <v>130</v>
-      </c>
-      <c r="D90" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>90</v>
-      </c>
-      <c r="B91" t="s">
-        <v>131</v>
-      </c>
-      <c r="C91" t="s">
-        <v>132</v>
-      </c>
-      <c r="D91" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>90</v>
-      </c>
-      <c r="B92" t="s">
-        <v>112</v>
-      </c>
-      <c r="C92" t="s">
-        <v>168</v>
-      </c>
-      <c r="D92" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>90</v>
-      </c>
-      <c r="B93" t="s">
-        <v>114</v>
-      </c>
-      <c r="C93" t="s">
-        <v>169</v>
-      </c>
-      <c r="D93" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>94</v>
-      </c>
-      <c r="B94" t="s">
-        <v>15</v>
-      </c>
-      <c r="C94" t="s">
-        <v>95</v>
-      </c>
-      <c r="D94" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>94</v>
-      </c>
-      <c r="B95" t="s">
-        <v>49</v>
-      </c>
-      <c r="C95" t="s">
-        <v>96</v>
-      </c>
-      <c r="D95" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>94</v>
-      </c>
-      <c r="B96" t="s">
-        <v>49</v>
-      </c>
-      <c r="C96" t="s">
-        <v>96</v>
-      </c>
-      <c r="D96" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>94</v>
-      </c>
-      <c r="B97" t="s">
-        <v>53</v>
-      </c>
-      <c r="C97" t="s">
-        <v>97</v>
-      </c>
-      <c r="D97" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>94</v>
-      </c>
-      <c r="B98" t="s">
-        <v>51</v>
-      </c>
-      <c r="C98" t="s">
-        <v>98</v>
-      </c>
-      <c r="D98" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>94</v>
-      </c>
-      <c r="B99" t="s">
-        <v>40</v>
-      </c>
-      <c r="C99" t="s">
-        <v>99</v>
-      </c>
-      <c r="D99" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>94</v>
-      </c>
-      <c r="B100" t="s">
-        <v>41</v>
-      </c>
-      <c r="C100" t="s">
-        <v>99</v>
-      </c>
-      <c r="D100" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>94</v>
-      </c>
-      <c r="B101" t="s">
-        <v>15</v>
-      </c>
-      <c r="C101" t="s">
-        <v>100</v>
-      </c>
-      <c r="D101" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>94</v>
-      </c>
-      <c r="B102" t="s">
-        <v>13</v>
-      </c>
-      <c r="C102" t="s">
-        <v>101</v>
-      </c>
-      <c r="D102" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>94</v>
-      </c>
-      <c r="B103" t="s">
-        <v>113</v>
-      </c>
-      <c r="C103" t="s">
-        <v>170</v>
-      </c>
-      <c r="D103" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>94</v>
-      </c>
-      <c r="B104" t="s">
-        <v>140</v>
-      </c>
-      <c r="C104" t="s">
-        <v>183</v>
-      </c>
-      <c r="D104" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>94</v>
-      </c>
-      <c r="B105" t="s">
-        <v>140</v>
-      </c>
-      <c r="C105" t="s">
-        <v>184</v>
-      </c>
-      <c r="D105" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>94</v>
-      </c>
-      <c r="B106" t="s">
-        <v>141</v>
-      </c>
-      <c r="C106" t="s">
-        <v>171</v>
-      </c>
-      <c r="D106" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>94</v>
-      </c>
-      <c r="B107" t="s">
-        <v>137</v>
-      </c>
-      <c r="C107" t="s">
-        <v>172</v>
-      </c>
-      <c r="D107" t="s">
-        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -4052,17 +2577,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="139fca70-673f-44e1-94c2-b523bb9c108c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7eaf932d-7370-48c5-9459-ae540daf9d7d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DFB9E5947890A84F90C1025035B3A9E9" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0fe1b0914d5c8b09183d39f4cd0f7192">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="139fca70-673f-44e1-94c2-b523bb9c108c" xmlns:ns3="7eaf932d-7370-48c5-9459-ae540daf9d7d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="356422204f896a562ca62bf92a067cf0" ns2:_="" ns3:_="">
     <xsd:import namespace="139fca70-673f-44e1-94c2-b523bb9c108c"/>
@@ -4269,6 +2783,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="139fca70-673f-44e1-94c2-b523bb9c108c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7eaf932d-7370-48c5-9459-ae540daf9d7d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -4279,23 +2804,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B57CF69-5D19-450C-935B-68EC43A8DA31}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="139fca70-673f-44e1-94c2-b523bb9c108c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="7eaf932d-7370-48c5-9459-ae540daf9d7d"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42A97454-B7ED-4BA8-A1AC-B982151F7AF7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4314,6 +2822,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B57CF69-5D19-450C-935B-68EC43A8DA31}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="139fca70-673f-44e1-94c2-b523bb9c108c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="7eaf932d-7370-48c5-9459-ae540daf9d7d"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BB2BB8B-BA4E-4835-AC34-431A62162A7D}">
   <ds:schemaRefs>

</xml_diff>